<commit_message>
firs version of run_multiple_scenarios_domain_reduction is running
</commit_message>
<xml_diff>
--- a/models/rfep elements.xlsx
+++ b/models/rfep elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="465" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD23E716-B717-4F4B-933C-A6B6C474D18C}"/>
+  <xr:revisionPtr revIDLastSave="480" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D01010D5-68BD-4D19-B682-9D37ABF84B8C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model elements" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId18"/>
+    <pivotCache cacheId="1" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="315">
   <si>
     <t>sets</t>
   </si>
@@ -1060,6 +1060,12 @@
   </si>
   <si>
     <t>value 2</t>
+  </si>
+  <si>
+    <t>timeLimit</t>
+  </si>
+  <si>
+    <t>value in call 2</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1417,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4AFB1DEB-AD54-432D-A639-8D2CCF6D6D22}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4AFB1DEB-AD54-432D-A639-8D2CCF6D6D22}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="G1:H4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -1733,8 +1739,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView showGridLines="0" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,10 +3033,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B35F91-3CD2-4C06-9BDF-CB9DD17C3DF6}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C70" sqref="C5:C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,26 +3089,24 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="str">
-        <f>"data_rfep["&amp;$B$3&amp;A5&amp;$B$3&amp;"]"</f>
-        <v>data_rfep["sNodesVehiclesPaths"]</v>
+      <c r="B5" s="30" t="s">
+        <v>109</v>
       </c>
       <c r="C5" s="6" t="str">
         <f>A5&amp;" = " &amp;B5&amp;","</f>
-        <v>sNodesVehiclesPaths = data_rfep["sNodesVehiclesPaths"],</v>
+        <v>sNodesVehiclesPaths = sNodesVehiclesPaths2,</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="30" t="str">
-        <f t="shared" ref="B6:B40" si="0">"data_rfep["&amp;$B$3&amp;A6&amp;$B$3&amp;"]"</f>
-        <v>data_rfep["sStationsVehiclesPaths"]</v>
+      <c r="B6" s="30" t="s">
+        <v>110</v>
       </c>
       <c r="C6" s="6" t="str">
-        <f t="shared" ref="C6:C20" si="1">A6&amp;" = " &amp;B6&amp;","</f>
-        <v>sStationsVehiclesPaths = data_rfep["sStationsVehiclesPaths"],</v>
+        <f t="shared" ref="C6:C20" si="0">A6&amp;" = " &amp;B6&amp;","</f>
+        <v>sStationsVehiclesPaths = sStationsVehiclesPaths2,</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3110,11 +3114,11 @@
         <v>3</v>
       </c>
       <c r="B7" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B6:B40" si="1">"data_rfep["&amp;$B$3&amp;A7&amp;$B$3&amp;"]"</f>
         <v>data_rfep["sOriginalStationsOwn"]</v>
       </c>
       <c r="C7" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sOriginalStationsOwn = data_rfep["sOriginalStationsOwn"],</v>
       </c>
     </row>
@@ -3123,11 +3127,11 @@
         <v>4</v>
       </c>
       <c r="B8" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sOriginalStationsPotential"]</v>
       </c>
       <c r="C8" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sOriginalStationsPotential = data_rfep["sOriginalStationsPotential"],</v>
       </c>
     </row>
@@ -3136,11 +3140,11 @@
         <v>5</v>
       </c>
       <c r="B9" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sSuppliers"]</v>
       </c>
       <c r="C9" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sSuppliers = data_rfep["sSuppliers"],</v>
       </c>
     </row>
@@ -3149,11 +3153,11 @@
         <v>6</v>
       </c>
       <c r="B10" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sSuppliersRanges"]</v>
       </c>
       <c r="C10" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sSuppliersRanges = data_rfep["sSuppliersRanges"],</v>
       </c>
     </row>
@@ -3162,11 +3166,11 @@
         <v>7</v>
       </c>
       <c r="B11" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sOriginVehiclesPaths"]</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sOriginVehiclesPaths = data_rfep["sOriginVehiclesPaths"],</v>
       </c>
     </row>
@@ -3175,11 +3179,11 @@
         <v>8</v>
       </c>
       <c r="B12" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sDestinationVehiclesPaths"]</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sDestinationVehiclesPaths = data_rfep["sDestinationVehiclesPaths"],</v>
       </c>
     </row>
@@ -3187,52 +3191,48 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>data_rfep["sSequenceNodesNodesVehiclesPaths"]</v>
+      <c r="B13" s="30" t="s">
+        <v>111</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>sSequenceNodesNodesVehiclesPaths = data_rfep["sSequenceNodesNodesVehiclesPaths"],</v>
+        <f t="shared" si="0"/>
+        <v>sSequenceNodesNodesVehiclesPaths = sSequenceNodesNodesVehiclesPaths2,</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>data_rfep["sFirstStationVehiclesPaths"]</v>
+      <c r="B14" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>sFirstStationVehiclesPaths = data_rfep["sFirstStationVehiclesPaths"],</v>
+        <f t="shared" si="0"/>
+        <v>sFirstStationVehiclesPaths = sFirstStationVehiclesPaths2,</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>data_rfep["sNotFirstStationVehiclesPaths"]</v>
+      <c r="B15" s="30" t="s">
+        <v>113</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>sNotFirstStationVehiclesPaths = data_rfep["sNotFirstStationVehiclesPaths"],</v>
+        <f t="shared" si="0"/>
+        <v>sNotFirstStationVehiclesPaths = sNotFirstStationVehiclesPaths2,</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>data_rfep["sNodesPotentialNodesOriginalVehiclesPaths"]</v>
+      <c r="B16" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="C16" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>sNodesPotentialNodesOriginalVehiclesPaths = data_rfep["sNodesPotentialNodesOriginalVehiclesPaths"],</v>
+        <f t="shared" si="0"/>
+        <v>sNodesPotentialNodesOriginalVehiclesPaths = sNodesPotentialNodesOriginalVehiclesPaths2,</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3240,11 +3240,11 @@
         <v>13</v>
       </c>
       <c r="B17" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sOriginalStationsMirrorStations"]</v>
       </c>
       <c r="C17" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sOriginalStationsMirrorStations = data_rfep["sOriginalStationsMirrorStations"],</v>
       </c>
     </row>
@@ -3253,11 +3253,11 @@
         <v>14</v>
       </c>
       <c r="B18" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sStationsSuppliers"]</v>
       </c>
       <c r="C18" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sStationsSuppliers = data_rfep["sStationsSuppliers"],</v>
       </c>
     </row>
@@ -3266,11 +3266,11 @@
         <v>15</v>
       </c>
       <c r="B19" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sSuppliersWithDiscount"]</v>
       </c>
       <c r="C19" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sSuppliersWithDiscount = data_rfep["sSuppliersWithDiscount"],</v>
       </c>
     </row>
@@ -3279,11 +3279,11 @@
         <v>69</v>
       </c>
       <c r="B20" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["sRanges"]</v>
       </c>
       <c r="C20" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>sRanges = data_rfep["sRanges"],</v>
       </c>
     </row>
@@ -3292,7 +3292,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pStartInventory"]</v>
       </c>
       <c r="C21" s="6" t="str">
@@ -3305,7 +3305,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pTargetInventory"]</v>
       </c>
       <c r="C22" s="6" t="str">
@@ -3318,7 +3318,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pSafetyStock"]</v>
       </c>
       <c r="C23" s="6" t="str">
@@ -3331,7 +3331,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pTankCapacity"]</v>
       </c>
       <c r="C24" s="6" t="str">
@@ -3344,7 +3344,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pMinRefuel"]</v>
       </c>
       <c r="C25" s="6" t="str">
@@ -3356,13 +3356,12 @@
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>data_rfep["pConsumptionMainRoute"]</v>
+      <c r="B26" s="30" t="s">
+        <v>115</v>
       </c>
       <c r="C26" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>pConsumptionMainRoute = data_rfep["pConsumptionMainRoute"],</v>
+        <v>pConsumptionMainRoute = pConsumptionMainRoute2,</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3370,7 +3369,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pConsumptionOOP"]</v>
       </c>
       <c r="C27" s="6" t="str">
@@ -3383,7 +3382,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pQuantityVehicles"]</v>
       </c>
       <c r="C28" s="6" t="str">
@@ -3396,7 +3395,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pStationCapacity"]</v>
       </c>
       <c r="C29" s="6" t="str">
@@ -3409,7 +3408,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pStationUnitCapacity"]</v>
       </c>
       <c r="C30" s="6" t="str">
@@ -3422,7 +3421,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pMinimumPurchaseQuantity"]</v>
       </c>
       <c r="C31" s="6" t="str">
@@ -3435,7 +3434,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pLowerQuantityDiscount"]</v>
       </c>
       <c r="C32" s="6" t="str">
@@ -3448,7 +3447,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pUpperQuantityDiscount"]</v>
       </c>
       <c r="C33" s="6" t="str">
@@ -3461,7 +3460,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pPrice"]</v>
       </c>
       <c r="C34" s="6" t="str">
@@ -3474,7 +3473,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pOpportunityCost"]</v>
       </c>
       <c r="C35" s="6" t="str">
@@ -3487,7 +3486,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pVariableCost"]</v>
       </c>
       <c r="C36" s="6" t="str">
@@ -3500,7 +3499,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pDistanceOOP"]</v>
       </c>
       <c r="C37" s="6" t="str">
@@ -3513,7 +3512,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pCostUnitCapacity"]</v>
       </c>
       <c r="C38" s="6" t="str">
@@ -3526,7 +3525,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pDiscount"]</v>
       </c>
       <c r="C39" s="6" t="str">
@@ -3539,7 +3538,7 @@
         <v>68</v>
       </c>
       <c r="B40" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>data_rfep["pLocationCost"]</v>
       </c>
       <c r="C40" s="6" t="str">
@@ -3569,7 +3568,7 @@
         <v>True</v>
       </c>
       <c r="C42" s="6" t="str">
-        <f t="shared" ref="C42:C69" si="4">"isON"&amp;A42&amp;" = "&amp;B42&amp;","</f>
+        <f t="shared" ref="C42:C70" si="4">"isON"&amp;A42&amp;" = "&amp;B42&amp;","</f>
         <v>isONvRefuelQuantity = True,</v>
       </c>
     </row>
@@ -3922,6 +3921,18 @@
       <c r="C69" s="6" t="str">
         <f t="shared" si="4"/>
         <v>isONtotalDiscount = True,</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B70">
+        <v>3600</v>
+      </c>
+      <c r="C70" s="6" t="str">
+        <f t="shared" ref="C70" si="5">A70&amp;" = " &amp;B70&amp;","</f>
+        <v>timeLimit = 3600,</v>
       </c>
     </row>
   </sheetData>
@@ -4022,7 +4033,7 @@
       </c>
       <c r="C5">
         <f ca="1">RAND()</f>
-        <v>0.42478492486444652</v>
+        <v>0.51130631381093927</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4034,7 +4045,7 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C7" ca="1" si="0">RAND()</f>
-        <v>0.42079253557585372</v>
+        <v>8.3017717448874984E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4046,7 +4057,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1575812662365218</v>
+        <v>0.7825536960310473</v>
       </c>
     </row>
   </sheetData>
@@ -4073,10 +4084,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7958CFEE-249C-447C-B869-76486DCAFC59}">
   <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4086,10 +4097,9 @@
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -4100,7 +4110,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -4116,8 +4126,11 @@
       <c r="E2" s="20" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="20" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>127</v>
       </c>
@@ -4133,14 +4146,8 @@
         <f>A3&amp;" = "&amp;D3&amp;","</f>
         <v>excel_input_file = file,</v>
       </c>
-      <c r="G3" t="s">
-        <v>109</v>
-      </c>
-      <c r="J3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>128</v>
       </c>
@@ -4156,14 +4163,8 @@
         <f>A4&amp;" = "&amp;D4&amp;","</f>
         <v>excel_output_file = output_file,</v>
       </c>
-      <c r="G4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>117</v>
       </c>
@@ -4179,14 +4180,8 @@
         <f t="shared" ref="E5:E34" si="1">A5&amp;" = "&amp;D5&amp;","</f>
         <v>scenario_name = scenario_name,</v>
       </c>
-      <c r="G5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>118</v>
       </c>
@@ -4202,14 +4197,8 @@
         <f t="shared" si="1"/>
         <v>output_solve = output_rfep,</v>
       </c>
-      <c r="G6" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>125</v>
       </c>
@@ -4227,14 +4216,8 @@
         <f t="shared" si="1"/>
         <v>total_time = total_time,</v>
       </c>
-      <c r="G7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>137</v>
       </c>
@@ -4254,14 +4237,8 @@
         <f t="shared" si="1"/>
         <v>b_domain_reduction = False,</v>
       </c>
-      <c r="G8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>138</v>
       </c>
@@ -4281,14 +4258,8 @@
         <f t="shared" si="1"/>
         <v>b_print_solution_detail = True,</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="J9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>161</v>
       </c>
@@ -4309,7 +4280,7 @@
         <v>b_print_location = True,</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>160</v>
       </c>
@@ -4330,7 +4301,7 @@
         <v>b_print_statistics = True,</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>130</v>
       </c>
@@ -4349,11 +4320,8 @@
         <f t="shared" si="1"/>
         <v>sVehiclesPaths = data_rfep["sVehiclesPaths"],</v>
       </c>
-      <c r="J12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
@@ -4372,11 +4340,8 @@
         <f t="shared" si="1"/>
         <v>sOriginalStationsPotential = data_rfep["sOriginalStationsPotential"],</v>
       </c>
-      <c r="J13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>9</v>
       </c>
@@ -4395,11 +4360,8 @@
         <f t="shared" si="1"/>
         <v>sSequenceNodesNodesVehiclesPaths = data_rfep["sSequenceNodesNodesVehiclesPaths"],</v>
       </c>
-      <c r="J14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>119</v>
       </c>
@@ -4418,11 +4380,8 @@
         <f t="shared" si="1"/>
         <v>sStationsPaths = data_rfep["sStationsPaths"],</v>
       </c>
-      <c r="J15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>3</v>
       </c>
@@ -4441,11 +4400,8 @@
         <f t="shared" si="1"/>
         <v>sOriginalStationsOwn = data_rfep["sOriginalStationsOwn"],</v>
       </c>
-      <c r="J16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>2</v>
       </c>
@@ -4464,11 +4420,8 @@
         <f t="shared" si="1"/>
         <v>sStationsVehiclesPaths = data_rfep["sStationsVehiclesPaths"],</v>
       </c>
-      <c r="J17" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>6</v>
       </c>
@@ -4487,11 +4440,8 @@
         <f t="shared" si="1"/>
         <v>sSuppliersRanges = data_rfep["sSuppliersRanges"],</v>
       </c>
-      <c r="J18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>17</v>
       </c>
@@ -4510,11 +4460,8 @@
         <f t="shared" si="1"/>
         <v>pStartInventory = data_rfep["pStartInventory"],</v>
       </c>
-      <c r="J19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>122</v>
       </c>
@@ -4533,11 +4480,8 @@
         <f t="shared" si="1"/>
         <v>pConsumptionRate = data_rfep["pConsumptionRate"],</v>
       </c>
-      <c r="J20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
         <v>123</v>
       </c>
@@ -4556,11 +4500,8 @@
         <f t="shared" si="1"/>
         <v>pDistance = data_rfep["pDistance"],</v>
       </c>
-      <c r="J21" s="22" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
         <v>126</v>
       </c>
@@ -4576,11 +4517,8 @@
         <v>data_rfep["pSubDistance"]</v>
       </c>
       <c r="E22" s="22"/>
-      <c r="J22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>22</v>
       </c>
@@ -4599,11 +4537,8 @@
         <f t="shared" si="1"/>
         <v>pConsumptionMainRoute = data_rfep["pConsumptionMainRoute"],</v>
       </c>
-      <c r="J23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
         <v>33</v>
       </c>
@@ -4622,11 +4557,8 @@
         <f t="shared" si="1"/>
         <v>pDistanceOOP = data_rfep["pDistanceOOP"],</v>
       </c>
-      <c r="J24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
         <v>23</v>
       </c>
@@ -4645,11 +4577,8 @@
         <f t="shared" si="1"/>
         <v>pConsumptionOOP = data_rfep["pConsumptionOOP"],</v>
       </c>
-      <c r="J25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>24</v>
       </c>
@@ -4669,7 +4598,7 @@
         <v>pQuantityVehicles = data_rfep["pQuantityVehicles"],</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>32</v>
       </c>
@@ -4689,7 +4618,7 @@
         <v>pVariableCost = data_rfep["pVariableCost"],</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>31</v>
       </c>
@@ -4709,7 +4638,7 @@
         <v>pOpportunityCost = data_rfep["pOpportunityCost"],</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>68</v>
       </c>
@@ -4729,7 +4658,7 @@
         <v>pLocationCost = data_rfep["pLocationCost"],</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>25</v>
       </c>
@@ -4749,7 +4678,7 @@
         <v>pStationCapacity = data_rfep["pStationCapacity"],</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>26</v>
       </c>
@@ -4769,7 +4698,7 @@
         <v>pStationUnitCapacity = data_rfep["pStationUnitCapacity"],</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
         <v>34</v>
       </c>
@@ -6072,7 +6001,7 @@
   <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8250,8 +8179,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="G36" sqref="G6:G36"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10398,12 +10327,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10602,27 +10531,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10647,9 +10567,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
export function for scenario stats
</commit_message>
<xml_diff>
--- a/models/rfep elements.xlsx
+++ b/models/rfep elements.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="500" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{476B6EB2-4FBC-428B-8972-2151407D4DDE}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAC26ED-71A8-41EE-A343-0D8EE02E2FA0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model elements" sheetId="1" r:id="rId1"/>
     <sheet name="rfep after domain reduction" sheetId="3" r:id="rId2"/>
     <sheet name="output subproblem" sheetId="2" r:id="rId3"/>
     <sheet name="Print Solution Function" sheetId="4" r:id="rId4"/>
-    <sheet name="Domain reduction function" sheetId="6" r:id="rId5"/>
-    <sheet name="Function Read instance" sheetId="9" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId7"/>
+    <sheet name="rfep_output_readability" sheetId="21" r:id="rId5"/>
+    <sheet name="Domain reduction function" sheetId="6" r:id="rId6"/>
+    <sheet name="Function Read instance" sheetId="9" r:id="rId7"/>
     <sheet name="output subproblem readability" sheetId="5" r:id="rId8"/>
     <sheet name="output domain reduction" sheetId="8" r:id="rId9"/>
     <sheet name="solve_multiple_frvrp" sheetId="10" r:id="rId10"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="325">
   <si>
     <t>sets</t>
   </si>
@@ -536,69 +536,6 @@
     <t>b_print_solution_detail</t>
   </si>
   <si>
-    <t>excel_input_file = file,</t>
-  </si>
-  <si>
-    <t>excel_output_file = output_file,</t>
-  </si>
-  <si>
-    <t>scenario_name = scenario_name,</t>
-  </si>
-  <si>
-    <t>output_solve = d_subproblem_solution[e],</t>
-  </si>
-  <si>
-    <t>b_print_solution_detail = True,</t>
-  </si>
-  <si>
-    <t>sVehiclesPaths = sSubVehiclesPaths,</t>
-  </si>
-  <si>
-    <t>sOriginalStationsPotential = sOriginalStationsPotential,</t>
-  </si>
-  <si>
-    <t>sSequenceNodesNodesVehiclesPaths = sSubSequenceNodesNodesVehiclesPaths,</t>
-  </si>
-  <si>
-    <t>sStationsPaths = sStationsPaths2,</t>
-  </si>
-  <si>
-    <t>sOriginalStationsOwn = sOriginalStationsOwn,</t>
-  </si>
-  <si>
-    <t>sStationsVehiclesPaths = sSubStationsVehiclesPaths,</t>
-  </si>
-  <si>
-    <t>pStartInventory = pStartInventory,</t>
-  </si>
-  <si>
-    <t>pConsumptionRate = pConsumptionRate,</t>
-  </si>
-  <si>
-    <t>pConsumptionMainRoute = pConsumptionMainRoute,</t>
-  </si>
-  <si>
-    <t>pDistanceOOP = pDistanceOOP,</t>
-  </si>
-  <si>
-    <t>pConsumptionOOP = pConsumptionOOP,</t>
-  </si>
-  <si>
-    <t>pQuantityVehicles = pQuantityVehicles,</t>
-  </si>
-  <si>
-    <t>pVariableCost = pVariableCost,</t>
-  </si>
-  <si>
-    <t>pOpportunityCost = pOpportunityCost,</t>
-  </si>
-  <si>
-    <t>pPrice = pPrice,</t>
-  </si>
-  <si>
-    <t>pDistance = pDistance,</t>
-  </si>
-  <si>
     <t>b_print_statistics</t>
   </si>
   <si>
@@ -1044,6 +981,117 @@
   </si>
   <si>
     <t>1 run of each Mult-FRVRP</t>
+  </si>
+  <si>
+    <t>solution_algorithm</t>
+  </si>
+  <si>
+    <t>value in call2</t>
+  </si>
+  <si>
+    <t>call2</t>
+  </si>
+  <si>
+    <t>b_retrieve_solve_ouput</t>
+  </si>
+  <si>
+    <t>status,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovInventory,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovRefuelQuantity,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovRefuel,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovQuantityUnitsCapacity,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovLocate,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovQuantityPurchased,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovQuantityPurchasedRange,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ovPurchasedRange,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                oTotalRefuellingCost,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                oTotalLocationCost,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                oTotalDiscount,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                oTotalCost,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_constraints,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_variables,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_integer_variables,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_binary_variables,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                model_fingerprint,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                model_runtime,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                model_MIPGap,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                model_nodeCount,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                model_initial_gap,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                model_time_first_incumbent,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                osvRefuelQuantity,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                osvRefuel,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                osvQuantityUnitsCapacity,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                osvLocate,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                osvQuantityPurchasedRange,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_vehicles,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_paths,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_avg_stations_path,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n_candidate_locations</t>
+  </si>
+  <si>
+    <t>Output</t>
   </si>
 </sst>
 </file>
@@ -2461,12 +2509,12 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>90</v>
@@ -2925,7 +2973,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3779,7 +3827,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="B70">
         <v>3600</v>
@@ -3821,7 +3869,7 @@
         <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3841,7 +3889,7 @@
         <v>133</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3905,7 +3953,7 @@
         <v>output_solve,</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="E6" s="22" t="str">
         <f t="shared" si="1"/>
@@ -3975,7 +4023,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B10" s="14" t="str">
         <f>"False"</f>
@@ -3996,7 +4044,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="B11" s="14" t="str">
         <f>"False"</f>
@@ -4496,32 +4544,32 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="E1" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="C3" t="str">
         <f>$C$1&amp;B3</f>
@@ -4534,10 +4582,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C19" si="0">$C$1&amp;B4</f>
@@ -4550,10 +4598,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -4566,10 +4614,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -4582,10 +4630,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4598,10 +4646,10 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4614,7 +4662,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="B9" s="38" t="str">
         <f>A9</f>
@@ -4635,7 +4683,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B10" s="38" t="str">
         <f t="shared" ref="B10:B19" si="3">A10</f>
@@ -4656,7 +4704,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B11" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4677,7 +4725,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B12" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4704,7 +4752,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B13" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4725,7 +4773,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B14" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4746,7 +4794,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B15" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4767,7 +4815,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="B16" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4788,7 +4836,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="B17" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4809,7 +4857,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="B18" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4830,7 +4878,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="B19" s="38" t="str">
         <f t="shared" si="3"/>
@@ -4870,31 +4918,31 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="C2" t="str">
         <f>A3</f>
@@ -4911,10 +4959,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C36" si="0">A4</f>
@@ -4931,10 +4979,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -4951,10 +4999,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -4971,10 +5019,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -4991,10 +5039,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -5011,10 +5059,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -5031,10 +5079,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -5051,10 +5099,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -5071,10 +5119,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -5091,10 +5139,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -5111,10 +5159,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -5131,10 +5179,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -5151,10 +5199,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="B15" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
@@ -5171,10 +5219,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -5191,10 +5239,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -5211,10 +5259,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -5231,10 +5279,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="B19" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -5251,10 +5299,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -5271,10 +5319,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -5291,10 +5339,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="B22" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -5311,10 +5359,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="B23" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -5331,10 +5379,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="B24" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -5351,10 +5399,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="B25" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -5371,10 +5419,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="B26" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -5391,10 +5439,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="B27" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -5411,10 +5459,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="B28" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -5431,10 +5479,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="B29" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -5451,10 +5499,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -5471,10 +5519,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B31" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -5491,10 +5539,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B32" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -5511,10 +5559,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -5531,10 +5579,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B34" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="0"/>
@@ -5551,10 +5599,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="B35" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="0"/>
@@ -5571,10 +5619,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B36" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="0"/>
@@ -5591,7 +5639,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -5618,31 +5666,31 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="C2" t="str">
         <f>A2</f>
@@ -5659,10 +5707,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C4" si="0">A3</f>
@@ -5679,10 +5727,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -5699,7 +5747,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -5711,7 +5759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121D905D-4443-4D4F-BAC5-5F82C02E29B9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -5723,34 +5771,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -7194,10 +7242,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7207,10 +7255,11 @@
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -7218,7 +7267,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -7234,8 +7283,14 @@
       <c r="E2" s="20" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>127</v>
       </c>
@@ -7248,17 +7303,18 @@
         <v>129</v>
       </c>
       <c r="E3" s="22" t="str">
-        <f>A3&amp;" = "&amp;D3&amp;","</f>
+        <f>$A3&amp;" = "&amp;D3&amp;","</f>
         <v>excel_input_file = file,</v>
       </c>
-      <c r="G3" t="s">
-        <v>109</v>
-      </c>
-      <c r="J3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="22" t="str">
+        <f>$A3&amp;" = "&amp;F3&amp;","</f>
+        <v>excel_input_file = file,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>128</v>
       </c>
@@ -7274,660 +7330,857 @@
         <f>A4&amp;" = "&amp;D4&amp;","</f>
         <v>excel_output_file = output_file,</v>
       </c>
-      <c r="G4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F4" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="22" t="str">
+        <f t="shared" ref="G4:G36" si="0">$A4&amp;" = "&amp;F4&amp;","</f>
+        <v>excel_output_file = output_file,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>117</v>
+        <v>288</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="22" t="str">
-        <f t="shared" ref="C5:C34" si="0">IF(B5="",A5&amp;",",A5&amp;"="&amp; B5&amp;",")</f>
-        <v>scenario_name,</v>
+        <f>IF(B5="",A5&amp;",",A5&amp;"="&amp; B5&amp;",")</f>
+        <v>solution_algorithm,</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" s="22" t="str">
+        <f>A5&amp;" = "&amp;D5&amp;","</f>
+        <v>solution_algorithm = solution_algorithm,</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>solution_algorithm = solution_algorithm,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>117</v>
-      </c>
-      <c r="E5" s="22" t="str">
-        <f t="shared" ref="E5:E34" si="1">A5&amp;" = "&amp;D5&amp;","</f>
-        <v>scenario_name = scenario_name,</v>
-      </c>
-      <c r="G5" t="s">
-        <v>111</v>
-      </c>
-      <c r="J5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>118</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C6:C36" si="1">IF(B6="",A6&amp;",",A6&amp;"="&amp; B6&amp;",")</f>
+        <v>scenario_name,</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="22" t="str">
+        <f t="shared" ref="E6:E36" si="2">A6&amp;" = "&amp;D6&amp;","</f>
+        <v>scenario_name = scenario_name,</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>scenario_name = scenario_name,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="22" t="str">
+        <f t="shared" si="1"/>
         <v>output_solve,</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" s="22" t="str">
-        <f t="shared" si="1"/>
+      <c r="D7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="22" t="str">
+        <f t="shared" si="2"/>
         <v>output_solve = output_rfep,</v>
       </c>
-      <c r="G6" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="F7" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>output_solve = output_rfep,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B8" s="14">
         <v>0</v>
       </c>
-      <c r="C7" s="22" t="str">
-        <f t="shared" si="0"/>
+      <c r="C8" s="22" t="str">
+        <f t="shared" si="1"/>
         <v>total_time=0,</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D8" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="22" t="str">
-        <f t="shared" si="1"/>
+      <c r="E8" s="22" t="str">
+        <f t="shared" si="2"/>
         <v>total_time = total_time,</v>
       </c>
-      <c r="G7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="F8" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>total_time = total_time,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="B8" s="14" t="str">
-        <f>"False"</f>
-        <v>False</v>
-      </c>
-      <c r="C8" s="22" t="str">
-        <f>IF(B8="",A8&amp;",",A8&amp;"="&amp; B8&amp;",")</f>
-        <v>b_domain_reduction=False,</v>
-      </c>
-      <c r="D8" s="14" t="str">
-        <f>"False"</f>
-        <v>False</v>
-      </c>
-      <c r="E8" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>b_domain_reduction = False,</v>
-      </c>
-      <c r="G8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>138</v>
       </c>
       <c r="B9" s="14" t="str">
         <f>"False"</f>
         <v>False</v>
       </c>
       <c r="C9" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>b_print_solution_detail=False,</v>
+        <f>IF(B9="",A9&amp;",",A9&amp;"="&amp; B9&amp;",")</f>
+        <v>b_domain_reduction=False,</v>
       </c>
       <c r="D9" s="14" t="str">
-        <f>"True"</f>
-        <v>True</v>
+        <f>"False"</f>
+        <v>False</v>
       </c>
       <c r="E9" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>b_print_solution_detail = True,</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="J9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>b_domain_reduction = False,</v>
+      </c>
+      <c r="F9" s="14" t="str">
+        <f>"False"</f>
+        <v>False</v>
+      </c>
+      <c r="G9" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>b_domain_reduction = False,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="B10" s="14" t="str">
         <f>"False"</f>
         <v>False</v>
       </c>
       <c r="C10" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>b_print_location=False,</v>
+        <f t="shared" si="1"/>
+        <v>b_print_solution_detail=False,</v>
       </c>
       <c r="D10" s="14" t="str">
         <f>"True"</f>
         <v>True</v>
       </c>
       <c r="E10" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>b_print_location = True,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>b_print_solution_detail = True,</v>
+      </c>
+      <c r="F10" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="G10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>b_print_solution_detail = True,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B11" s="14" t="str">
         <f>"False"</f>
         <v>False</v>
       </c>
       <c r="C11" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>b_print_statistics=False,</v>
+        <f t="shared" si="1"/>
+        <v>b_print_location=False,</v>
       </c>
       <c r="D11" s="14" t="str">
         <f>"True"</f>
         <v>True</v>
       </c>
       <c r="E11" s="22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>b_print_location = True,</v>
+      </c>
+      <c r="F11" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="G11" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>b_print_location = True,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="14" t="str">
+        <f>"False"</f>
+        <v>False</v>
+      </c>
+      <c r="C12" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>b_print_statistics=False,</v>
+      </c>
+      <c r="D12" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="E12" s="22" t="str">
+        <f t="shared" si="2"/>
         <v>b_print_statistics = True,</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="F12" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="G12" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>b_print_statistics = True,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="C13" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>b_retrieve_solve_ouput=True,</v>
+      </c>
+      <c r="D13" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="E13" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>b_retrieve_solve_ouput = True,</v>
+      </c>
+      <c r="F13" s="14" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="G13" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>b_retrieve_solve_ouput = True,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>130</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sVehiclesPaths=[],</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sVehiclesPaths = sVehiclesPaths,</v>
-      </c>
-      <c r="J12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sOriginalStationsPotential=[],</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sOriginalStationsPotential = sOriginalStationsPotential,</v>
-      </c>
-      <c r="J13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>9</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>121</v>
       </c>
       <c r="C14" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sSequenceNodesNodesVehiclesPaths=[],</v>
+        <f t="shared" si="1"/>
+        <v>sVehiclesPaths=[],</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="E14" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sSequenceNodesNodesVehiclesPaths = sSequenceNodesNodesVehiclesPaths2,</v>
-      </c>
-      <c r="J14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>119</v>
+        <f t="shared" si="2"/>
+        <v>sVehiclesPaths = sVehiclesPaths,</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sVehiclesPaths = sVehiclesPaths,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C15" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sStationsPaths=set(),</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>136</v>
+        <f t="shared" si="1"/>
+        <v>sOriginalStationsPotential=[],</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>4</v>
       </c>
       <c r="E15" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sStationsPaths = sStationsPaths2,</v>
-      </c>
-      <c r="J15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>sOriginalStationsPotential = sOriginalStationsPotential,</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sOriginalStationsPotential = sOriginalStationsPotential,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>121</v>
       </c>
       <c r="C16" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sOriginalStationsOwn=[],</v>
+        <f t="shared" si="1"/>
+        <v>sSequenceNodesNodesVehiclesPaths=[],</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="E16" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sOriginalStationsOwn = sOriginalStationsOwn,</v>
-      </c>
-      <c r="J16" t="s">
-        <v>150</v>
+        <f t="shared" si="2"/>
+        <v>sSequenceNodesNodesVehiclesPaths = sSequenceNodesNodesVehiclesPaths2,</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sSequenceNodesNodesVehiclesPaths = sSequenceNodesNodesVehiclesPaths,</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C17" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sStationsVehiclesPaths=[],</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>110</v>
+        <f t="shared" si="1"/>
+        <v>sStationsPaths=set(),</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>136</v>
       </c>
       <c r="E17" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sStationsVehiclesPaths = sStationsVehiclesPaths2,</v>
-      </c>
-      <c r="J17" t="s">
-        <v>151</v>
+        <f t="shared" si="2"/>
+        <v>sStationsPaths = sStationsPaths2,</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sStationsPaths = sStationsPaths,</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>121</v>
       </c>
       <c r="C18" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>sSuppliersRanges=[],</v>
-      </c>
-      <c r="D18" s="21" t="str">
-        <f>A18</f>
-        <v>sSuppliersRanges</v>
+        <f t="shared" si="1"/>
+        <v>sOriginalStationsOwn=[],</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="E18" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>sSuppliersRanges = sSuppliersRanges,</v>
-      </c>
-      <c r="J18" t="s">
-        <v>152</v>
+        <f t="shared" si="2"/>
+        <v>sOriginalStationsOwn = sOriginalStationsOwn,</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sOriginalStationsOwn = sOriginalStationsOwn,</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="14">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="C19" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pStartInventory=0,</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>17</v>
+        <f t="shared" si="1"/>
+        <v>sStationsVehiclesPaths=[],</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="E19" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pStartInventory = pStartInventory,</v>
-      </c>
-      <c r="J19" t="s">
-        <v>153</v>
+        <f t="shared" si="2"/>
+        <v>sStationsVehiclesPaths = sStationsVehiclesPaths2,</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sStationsVehiclesPaths = sStationsVehiclesPaths,</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="14">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>121</v>
       </c>
       <c r="C20" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pConsumptionRate=0,</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>122</v>
+        <f t="shared" si="1"/>
+        <v>sSuppliersRanges=[],</v>
+      </c>
+      <c r="D20" s="21" t="str">
+        <f>A20</f>
+        <v>sSuppliersRanges</v>
       </c>
       <c r="E20" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pConsumptionRate = pConsumptionRate,</v>
-      </c>
-      <c r="J20" t="s">
-        <v>154</v>
+        <f t="shared" si="2"/>
+        <v>sSuppliersRanges = sSuppliersRanges,</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>sSuppliersRanges = sSuppliersRanges,</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>123</v>
+        <v>17</v>
       </c>
       <c r="B21" s="14">
         <v>0</v>
       </c>
       <c r="C21" s="22" t="str">
-        <f>IF(B21="",A21&amp;",",A21&amp;"="&amp; B21&amp;",")</f>
-        <v>pDistance=0,</v>
+        <f t="shared" si="1"/>
+        <v>pStartInventory=0,</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="J21" s="22" t="s">
-        <v>159</v>
+        <v>17</v>
+      </c>
+      <c r="E21" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>pStartInventory = pStartInventory,</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pStartInventory = pStartInventory,</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B22" s="14">
         <v>0</v>
       </c>
       <c r="C22" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pSubDistance=0,</v>
-      </c>
-      <c r="D22" s="21" t="str">
-        <f>A22</f>
-        <v>pSubDistance</v>
+        <f t="shared" si="1"/>
+        <v>pConsumptionRate=0,</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="E22" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pSubDistance = pSubDistance,</v>
-      </c>
-      <c r="J22" t="s">
-        <v>155</v>
+        <f t="shared" si="2"/>
+        <v>pConsumptionRate = pConsumptionRate,</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G22" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pConsumptionRate = pConsumptionRate,</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
       </c>
       <c r="C23" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pConsumptionMainRoute=0,</v>
+        <f>IF(B23="",A23&amp;",",A23&amp;"="&amp; B23&amp;",")</f>
+        <v>pDistance=0,</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pConsumptionMainRoute = pConsumptionMainRoute2,</v>
-      </c>
-      <c r="J23" t="s">
-        <v>156</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="E23" s="22"/>
+      <c r="F23" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pDistance = pDistance,</v>
+      </c>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="B24" s="14">
         <v>0</v>
       </c>
       <c r="C24" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pDistanceOOP=0,</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>33</v>
+        <f t="shared" si="1"/>
+        <v>pSubDistance=0,</v>
+      </c>
+      <c r="D24" s="21" t="str">
+        <f>A24</f>
+        <v>pSubDistance</v>
       </c>
       <c r="E24" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pDistanceOOP = pDistanceOOP,</v>
-      </c>
-      <c r="J24" t="s">
-        <v>157</v>
+        <f t="shared" si="2"/>
+        <v>pSubDistance = pSubDistance,</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pSubDistance = pSubDistance,</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="14">
         <v>0</v>
       </c>
       <c r="C25" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pConsumptionOOP=0,</v>
+        <f t="shared" si="1"/>
+        <v>pConsumptionMainRoute=0,</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="E25" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pConsumptionOOP = pConsumptionOOP,</v>
-      </c>
-      <c r="J25" t="s">
-        <v>158</v>
+        <f t="shared" si="2"/>
+        <v>pConsumptionMainRoute = pConsumptionMainRoute2,</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pConsumptionMainRoute = pConsumptionMainRoute,</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B26" s="14">
         <v>0</v>
       </c>
       <c r="C26" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pQuantityVehicles=0,</v>
+        <f t="shared" si="1"/>
+        <v>pDistanceOOP=0,</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E26" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pQuantityVehicles = pQuantityVehicles,</v>
+        <f t="shared" si="2"/>
+        <v>pDistanceOOP = pDistanceOOP,</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pDistanceOOP = pDistanceOOP,</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B27" s="14">
         <v>0</v>
       </c>
       <c r="C27" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pVariableCost=0,</v>
+        <f t="shared" si="1"/>
+        <v>pConsumptionOOP=0,</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E27" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pVariableCost = pVariableCost,</v>
+        <f t="shared" si="2"/>
+        <v>pConsumptionOOP = pConsumptionOOP,</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pConsumptionOOP = pConsumptionOOP,</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B28" s="14">
         <v>0</v>
       </c>
       <c r="C28" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pOpportunityCost=0,</v>
+        <f t="shared" si="1"/>
+        <v>pQuantityVehicles=0,</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E28" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pOpportunityCost = pOpportunityCost,</v>
+        <f t="shared" si="2"/>
+        <v>pQuantityVehicles = pQuantityVehicles,</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pQuantityVehicles = pQuantityVehicles,</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B29" s="14">
         <v>0</v>
       </c>
       <c r="C29" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pLocationCost=0,</v>
-      </c>
-      <c r="D29" s="21" t="str">
-        <f t="shared" ref="D29:D31" si="2">A29</f>
-        <v>pLocationCost</v>
+        <f t="shared" si="1"/>
+        <v>pVariableCost=0,</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="E29" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pLocationCost = pLocationCost,</v>
+        <f t="shared" si="2"/>
+        <v>pVariableCost = pVariableCost,</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pVariableCost = pVariableCost,</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B30" s="14">
         <v>0</v>
       </c>
       <c r="C30" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pStationCapacity=0,</v>
-      </c>
-      <c r="D30" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>pStationCapacity</v>
+        <f t="shared" si="1"/>
+        <v>pOpportunityCost=0,</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="E30" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pStationCapacity = pStationCapacity,</v>
+        <f t="shared" si="2"/>
+        <v>pOpportunityCost = pOpportunityCost,</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pOpportunityCost = pOpportunityCost,</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="B31" s="14">
         <v>0</v>
       </c>
       <c r="C31" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pStationUnitCapacity=0,</v>
+        <f t="shared" si="1"/>
+        <v>pLocationCost=0,</v>
       </c>
       <c r="D31" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>pStationUnitCapacity</v>
+        <f t="shared" ref="D31:D33" si="3">A31</f>
+        <v>pLocationCost</v>
       </c>
       <c r="E31" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pStationUnitCapacity = pStationUnitCapacity,</v>
+        <f t="shared" si="2"/>
+        <v>pLocationCost = pLocationCost,</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pLocationCost = pLocationCost,</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B32" s="14">
         <v>0</v>
       </c>
       <c r="C32" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pCostUnitCapacity=0,</v>
+        <f t="shared" si="1"/>
+        <v>pStationCapacity=0,</v>
       </c>
       <c r="D32" s="21" t="str">
-        <f>A32</f>
-        <v>pCostUnitCapacity</v>
+        <f t="shared" si="3"/>
+        <v>pStationCapacity</v>
       </c>
       <c r="E32" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pCostUnitCapacity = pCostUnitCapacity,</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>pStationCapacity = pStationCapacity,</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pStationCapacity = pStationCapacity,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B33" s="14">
         <v>0</v>
       </c>
       <c r="C33" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pPrice=0,</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>pStationUnitCapacity=0,</v>
+      </c>
+      <c r="D33" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>pStationUnitCapacity</v>
       </c>
       <c r="E33" s="22" t="str">
-        <f t="shared" si="1"/>
-        <v>pPrice = pPrice,</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>pStationUnitCapacity = pStationUnitCapacity,</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pStationUnitCapacity = pStationUnitCapacity,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="14">
         <v>0</v>
       </c>
       <c r="C34" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>pDiscount=0,</v>
+        <f t="shared" si="1"/>
+        <v>pCostUnitCapacity=0,</v>
       </c>
       <c r="D34" s="21" t="str">
         <f>A34</f>
+        <v>pCostUnitCapacity</v>
+      </c>
+      <c r="E34" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>pCostUnitCapacity = pCostUnitCapacity,</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pCostUnitCapacity = pCostUnitCapacity,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="14">
+        <v>0</v>
+      </c>
+      <c r="C35" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>pPrice=0,</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>pPrice = pPrice,</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>pPrice = pPrice,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="14">
+        <v>0</v>
+      </c>
+      <c r="C36" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>pDiscount=0,</v>
+      </c>
+      <c r="D36" s="21" t="str">
+        <f>A36</f>
         <v>pDiscount</v>
       </c>
-      <c r="E34" s="22" t="str">
-        <f t="shared" si="1"/>
+      <c r="E36" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>pDiscount = pDiscount,</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" s="22" t="str">
+        <f t="shared" si="0"/>
         <v>pDiscount = pDiscount,</v>
       </c>
     </row>
@@ -7938,6 +8191,316 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54D8714-998C-4B41-905B-35650263B8F4}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A33" si="0">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G36"/>
@@ -7958,35 +8521,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="F2" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B3" s="23">
         <v>1</v>
@@ -8014,7 +8577,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B4" s="23">
         <v>2</v>
@@ -8042,7 +8605,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B5" s="23">
         <v>2</v>
@@ -8941,7 +9504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F43"/>
@@ -8959,21 +9522,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>70</v>
       </c>
       <c r="D1" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B2" t="str">
         <f>A2&amp;","</f>
@@ -8983,7 +9546,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="F2" t="str">
         <f>""""&amp;E2&amp;"""" &amp; ": "&amp;E2&amp;","</f>
@@ -8992,7 +9555,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B3" t="str">
         <f>A3&amp;","</f>
@@ -9008,7 +9571,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" ref="B4:B11" si="1">A4&amp;","</f>
@@ -9024,7 +9587,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="1"/>
@@ -9040,7 +9603,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
@@ -9056,7 +9619,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
@@ -9072,7 +9635,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
@@ -9088,7 +9651,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
@@ -9104,7 +9667,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
@@ -9120,7 +9683,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
@@ -9280,7 +9843,7 @@
     </row>
     <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -9425,19 +9988,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1772A6-DE71-443F-9056-9F78044A9E0F}">
-  <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9979,13 +10529,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10090,6 +10640,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8792194EFF3EC4B9DEDA9143FB158AB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74d6161c0732f6a6a47db9602d75fed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6d2cdb912d1a107b914756c6dc16714" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10284,25 +10852,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00C25CB2-CB7D-473C-8D2E-8B42FDF875CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10319,29 +10894,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
export_solution_rfep is esporting solution details
</commit_message>
<xml_diff>
--- a/models/rfep elements.xlsx
+++ b/models/rfep elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="565" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAC26ED-71A8-41EE-A343-0D8EE02E2FA0}"/>
+  <xr:revisionPtr revIDLastSave="574" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E98193C-2A42-4DB5-82F4-42653A1C473A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model elements" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="322">
   <si>
     <t>sets</t>
   </si>
@@ -1068,15 +1068,6 @@
   </si>
   <si>
     <t xml:space="preserve">                osvRefuel,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                osvQuantityUnitsCapacity,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                osvLocate,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                osvQuantityPurchasedRange,</t>
   </si>
   <si>
     <t xml:space="preserve">                n_vehicles,</t>
@@ -7244,8 +7235,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G36"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7599,12 +7590,13 @@
         <f t="shared" si="2"/>
         <v>sVehiclesPaths = sVehiclesPaths,</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>130</v>
+      <c r="F14" s="14" t="str">
+        <f>"data_rfep["""&amp;A14&amp;""&amp;""""&amp;"]"</f>
+        <v>data_rfep["sVehiclesPaths"]</v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sVehiclesPaths = sVehiclesPaths,</v>
+        <v>sVehiclesPaths = data_rfep["sVehiclesPaths"],</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -7625,12 +7617,13 @@
         <f t="shared" si="2"/>
         <v>sOriginalStationsPotential = sOriginalStationsPotential,</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>4</v>
+      <c r="F15" s="14" t="str">
+        <f t="shared" ref="F15:F36" si="3">"data_rfep["""&amp;A15&amp;""&amp;""""&amp;"]"</f>
+        <v>data_rfep["sOriginalStationsPotential"]</v>
       </c>
       <c r="G15" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sOriginalStationsPotential = sOriginalStationsPotential,</v>
+        <v>sOriginalStationsPotential = data_rfep["sOriginalStationsPotential"],</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -7651,12 +7644,13 @@
         <f t="shared" si="2"/>
         <v>sSequenceNodesNodesVehiclesPaths = sSequenceNodesNodesVehiclesPaths2,</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>9</v>
+      <c r="F16" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["sSequenceNodesNodesVehiclesPaths"]</v>
       </c>
       <c r="G16" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sSequenceNodesNodesVehiclesPaths = sSequenceNodesNodesVehiclesPaths,</v>
+        <v>sSequenceNodesNodesVehiclesPaths = data_rfep["sSequenceNodesNodesVehiclesPaths"],</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -7677,12 +7671,13 @@
         <f t="shared" si="2"/>
         <v>sStationsPaths = sStationsPaths2,</v>
       </c>
-      <c r="F17" s="21" t="s">
-        <v>119</v>
+      <c r="F17" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["sStationsPaths"]</v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sStationsPaths = sStationsPaths,</v>
+        <v>sStationsPaths = data_rfep["sStationsPaths"],</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -7703,12 +7698,13 @@
         <f t="shared" si="2"/>
         <v>sOriginalStationsOwn = sOriginalStationsOwn,</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>3</v>
+      <c r="F18" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["sOriginalStationsOwn"]</v>
       </c>
       <c r="G18" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sOriginalStationsOwn = sOriginalStationsOwn,</v>
+        <v>sOriginalStationsOwn = data_rfep["sOriginalStationsOwn"],</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -7729,12 +7725,13 @@
         <f t="shared" si="2"/>
         <v>sStationsVehiclesPaths = sStationsVehiclesPaths2,</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>2</v>
+      <c r="F19" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["sStationsVehiclesPaths"]</v>
       </c>
       <c r="G19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sStationsVehiclesPaths = sStationsVehiclesPaths,</v>
+        <v>sStationsVehiclesPaths = data_rfep["sStationsVehiclesPaths"],</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -7756,12 +7753,13 @@
         <f t="shared" si="2"/>
         <v>sSuppliersRanges = sSuppliersRanges,</v>
       </c>
-      <c r="F20" s="21" t="s">
-        <v>6</v>
+      <c r="F20" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["sSuppliersRanges"]</v>
       </c>
       <c r="G20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>sSuppliersRanges = sSuppliersRanges,</v>
+        <v>sSuppliersRanges = data_rfep["sSuppliersRanges"],</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -7782,12 +7780,13 @@
         <f t="shared" si="2"/>
         <v>pStartInventory = pStartInventory,</v>
       </c>
-      <c r="F21" s="21" t="s">
-        <v>17</v>
+      <c r="F21" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pStartInventory"]</v>
       </c>
       <c r="G21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pStartInventory = pStartInventory,</v>
+        <v>pStartInventory = data_rfep["pStartInventory"],</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -7808,12 +7807,13 @@
         <f t="shared" si="2"/>
         <v>pConsumptionRate = pConsumptionRate,</v>
       </c>
-      <c r="F22" s="21" t="s">
-        <v>122</v>
+      <c r="F22" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pConsumptionRate"]</v>
       </c>
       <c r="G22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pConsumptionRate = pConsumptionRate,</v>
+        <v>pConsumptionRate = data_rfep["pConsumptionRate"],</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -7831,12 +7831,13 @@
         <v>123</v>
       </c>
       <c r="E23" s="22"/>
-      <c r="F23" s="21" t="s">
-        <v>123</v>
+      <c r="F23" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pDistance"]</v>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pDistance = pDistance,</v>
+        <v>pDistance = data_rfep["pDistance"],</v>
       </c>
       <c r="J23" s="22"/>
     </row>
@@ -7859,12 +7860,13 @@
         <f t="shared" si="2"/>
         <v>pSubDistance = pSubDistance,</v>
       </c>
-      <c r="F24" s="21" t="s">
-        <v>126</v>
+      <c r="F24" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pSubDistance"]</v>
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pSubDistance = pSubDistance,</v>
+        <v>pSubDistance = data_rfep["pSubDistance"],</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7885,12 +7887,13 @@
         <f t="shared" si="2"/>
         <v>pConsumptionMainRoute = pConsumptionMainRoute2,</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>22</v>
+      <c r="F25" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pConsumptionMainRoute"]</v>
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pConsumptionMainRoute = pConsumptionMainRoute,</v>
+        <v>pConsumptionMainRoute = data_rfep["pConsumptionMainRoute"],</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -7911,12 +7914,13 @@
         <f t="shared" si="2"/>
         <v>pDistanceOOP = pDistanceOOP,</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>33</v>
+      <c r="F26" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pDistanceOOP"]</v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pDistanceOOP = pDistanceOOP,</v>
+        <v>pDistanceOOP = data_rfep["pDistanceOOP"],</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -7937,12 +7941,13 @@
         <f t="shared" si="2"/>
         <v>pConsumptionOOP = pConsumptionOOP,</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>23</v>
+      <c r="F27" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pConsumptionOOP"]</v>
       </c>
       <c r="G27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pConsumptionOOP = pConsumptionOOP,</v>
+        <v>pConsumptionOOP = data_rfep["pConsumptionOOP"],</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -7963,12 +7968,13 @@
         <f t="shared" si="2"/>
         <v>pQuantityVehicles = pQuantityVehicles,</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>24</v>
+      <c r="F28" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pQuantityVehicles"]</v>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pQuantityVehicles = pQuantityVehicles,</v>
+        <v>pQuantityVehicles = data_rfep["pQuantityVehicles"],</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -7989,12 +7995,13 @@
         <f t="shared" si="2"/>
         <v>pVariableCost = pVariableCost,</v>
       </c>
-      <c r="F29" s="21" t="s">
-        <v>32</v>
+      <c r="F29" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pVariableCost"]</v>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pVariableCost = pVariableCost,</v>
+        <v>pVariableCost = data_rfep["pVariableCost"],</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -8015,12 +8022,13 @@
         <f t="shared" si="2"/>
         <v>pOpportunityCost = pOpportunityCost,</v>
       </c>
-      <c r="F30" s="21" t="s">
-        <v>31</v>
+      <c r="F30" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pOpportunityCost"]</v>
       </c>
       <c r="G30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pOpportunityCost = pOpportunityCost,</v>
+        <v>pOpportunityCost = data_rfep["pOpportunityCost"],</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -8035,19 +8043,20 @@
         <v>pLocationCost=0,</v>
       </c>
       <c r="D31" s="21" t="str">
-        <f t="shared" ref="D31:D33" si="3">A31</f>
+        <f t="shared" ref="D31:D33" si="4">A31</f>
         <v>pLocationCost</v>
       </c>
       <c r="E31" s="22" t="str">
         <f t="shared" si="2"/>
         <v>pLocationCost = pLocationCost,</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>68</v>
+      <c r="F31" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pLocationCost"]</v>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pLocationCost = pLocationCost,</v>
+        <v>pLocationCost = data_rfep["pLocationCost"],</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -8062,19 +8071,20 @@
         <v>pStationCapacity=0,</v>
       </c>
       <c r="D32" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>pStationCapacity</v>
+      </c>
+      <c r="E32" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>pStationCapacity = pStationCapacity,</v>
+      </c>
+      <c r="F32" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>pStationCapacity</v>
-      </c>
-      <c r="E32" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>pStationCapacity = pStationCapacity,</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>25</v>
+        <v>data_rfep["pStationCapacity"]</v>
       </c>
       <c r="G32" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pStationCapacity = pStationCapacity,</v>
+        <v>pStationCapacity = data_rfep["pStationCapacity"],</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -8089,19 +8099,20 @@
         <v>pStationUnitCapacity=0,</v>
       </c>
       <c r="D33" s="21" t="str">
+        <f t="shared" si="4"/>
+        <v>pStationUnitCapacity</v>
+      </c>
+      <c r="E33" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v>pStationUnitCapacity = pStationUnitCapacity,</v>
+      </c>
+      <c r="F33" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>pStationUnitCapacity</v>
-      </c>
-      <c r="E33" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v>pStationUnitCapacity = pStationUnitCapacity,</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>26</v>
+        <v>data_rfep["pStationUnitCapacity"]</v>
       </c>
       <c r="G33" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pStationUnitCapacity = pStationUnitCapacity,</v>
+        <v>pStationUnitCapacity = data_rfep["pStationUnitCapacity"],</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -8123,12 +8134,13 @@
         <f t="shared" si="2"/>
         <v>pCostUnitCapacity = pCostUnitCapacity,</v>
       </c>
-      <c r="F34" s="21" t="s">
-        <v>34</v>
+      <c r="F34" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pCostUnitCapacity"]</v>
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pCostUnitCapacity = pCostUnitCapacity,</v>
+        <v>pCostUnitCapacity = data_rfep["pCostUnitCapacity"],</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -8149,12 +8161,13 @@
         <f t="shared" si="2"/>
         <v>pPrice = pPrice,</v>
       </c>
-      <c r="F35" s="21" t="s">
-        <v>30</v>
+      <c r="F35" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pPrice"]</v>
       </c>
       <c r="G35" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pPrice = pPrice,</v>
+        <v>pPrice = data_rfep["pPrice"],</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -8176,12 +8189,13 @@
         <f t="shared" si="2"/>
         <v>pDiscount = pDiscount,</v>
       </c>
-      <c r="F36" s="21" t="s">
-        <v>35</v>
+      <c r="F36" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>data_rfep["pDiscount"]</v>
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>pDiscount = pDiscount,</v>
+        <v>pDiscount = data_rfep["pDiscount"],</v>
       </c>
     </row>
   </sheetData>
@@ -8192,10 +8206,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54D8714-998C-4B41-905B-35650263B8F4}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8205,7 +8219,7 @@
         <v>148</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -8227,7 +8241,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A33" si="0">A3+1</f>
+        <f t="shared" ref="A4:A30" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -8466,33 +8480,6 @@
       </c>
       <c r="B30" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mip start feauture added to rfep
</commit_message>
<xml_diff>
--- a/models/rfep elements.xlsx
+++ b/models/rfep elements.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="574" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E98193C-2A42-4DB5-82F4-42653A1C473A}"/>
+  <xr:revisionPtr revIDLastSave="603" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{211BD5DB-49E1-401E-82F8-A0A5DC112343}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model elements" sheetId="1" r:id="rId1"/>
-    <sheet name="rfep after domain reduction" sheetId="3" r:id="rId2"/>
-    <sheet name="output subproblem" sheetId="2" r:id="rId3"/>
-    <sheet name="Print Solution Function" sheetId="4" r:id="rId4"/>
-    <sheet name="rfep_output_readability" sheetId="21" r:id="rId5"/>
-    <sheet name="Domain reduction function" sheetId="6" r:id="rId6"/>
-    <sheet name="Function Read instance" sheetId="9" r:id="rId7"/>
-    <sheet name="output subproblem readability" sheetId="5" r:id="rId8"/>
-    <sheet name="output domain reduction" sheetId="8" r:id="rId9"/>
-    <sheet name="solve_multiple_frvrp" sheetId="10" r:id="rId10"/>
-    <sheet name="rfep run experiments" sheetId="13" r:id="rId11"/>
-    <sheet name="Print Solution Experiments" sheetId="14" r:id="rId12"/>
-    <sheet name="Building factor combination" sheetId="15" r:id="rId13"/>
-    <sheet name="Tracking events data reading" sheetId="16" r:id="rId14"/>
-    <sheet name="Tracking events solve multiple" sheetId="17" r:id="rId15"/>
-    <sheet name="Solution Methodologies" sheetId="20" r:id="rId16"/>
+    <sheet name="mip_start" sheetId="22" r:id="rId2"/>
+    <sheet name="rfep after domain reduction" sheetId="3" r:id="rId3"/>
+    <sheet name="output subproblem" sheetId="2" r:id="rId4"/>
+    <sheet name="Print Solution Function" sheetId="4" r:id="rId5"/>
+    <sheet name="rfep_output_readability" sheetId="21" r:id="rId6"/>
+    <sheet name="Domain reduction function" sheetId="6" r:id="rId7"/>
+    <sheet name="Function Read instance" sheetId="9" r:id="rId8"/>
+    <sheet name="output subproblem readability" sheetId="5" r:id="rId9"/>
+    <sheet name="output domain reduction" sheetId="8" r:id="rId10"/>
+    <sheet name="solve_multiple_frvrp" sheetId="10" r:id="rId11"/>
+    <sheet name="rfep run experiments" sheetId="13" r:id="rId12"/>
+    <sheet name="Print Solution Experiments" sheetId="14" r:id="rId13"/>
+    <sheet name="Building factor combination" sheetId="15" r:id="rId14"/>
+    <sheet name="Tracking events data reading" sheetId="16" r:id="rId15"/>
+    <sheet name="Tracking events solve multiple" sheetId="17" r:id="rId16"/>
+    <sheet name="Solution Methodologies" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -117,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="322">
   <si>
     <t>sets</t>
   </si>
@@ -1632,8 +1633,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H16" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,6 +2461,133 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="str">
+        <f>B2&amp;"="&amp;$D$1&amp;"["&amp;A2&amp;"]"</f>
+        <v>sNodesVehiclesPaths2=output_domain_reduction[0]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D9" si="0">B3&amp;"="&amp;$D$1&amp;"["&amp;A3&amp;"]"</f>
+        <v>sStationsVehiclesPaths2=output_domain_reduction[1]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>sSequenceNodesNodesVehiclesPaths2=output_domain_reduction[2]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>sFirstStationVehiclesPaths2=output_domain_reduction[3]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>sNotFirstStationVehiclesPaths2=output_domain_reduction[4]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>sNodesPotentialNodesOriginalVehiclesPaths2=output_domain_reduction[5]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>pConsumptionMainRoute2=output_domain_reduction[6]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>sStationsPaths2=output_domain_reduction[7]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F26CE2-C90F-4A38-9A6A-C140B73B9CCE}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C35"/>
@@ -2923,7 +3051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B35F91-3CD2-4C06-9BDF-CB9DD17C3DF6}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C70"/>
@@ -3834,7 +3962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7958CFEE-249C-447C-B869-76486DCAFC59}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:F34"/>
@@ -4517,7 +4645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F78C82-2E64-4261-A67D-49932A4E459B}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:O19"/>
@@ -4893,7 +5021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CF5A27-5F77-4909-AEA0-BD4A0A79DDCF}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:G37"/>
@@ -5638,7 +5766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F50D163-8D8F-40C3-B1E6-F806996DCA94}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:G5"/>
@@ -5746,7 +5874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121D905D-4443-4D4F-BAC5-5F82C02E29B9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5798,6 +5926,385 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C04E18-08DD-4053-843A-816A92C25787}">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"mip_start["&amp;$C$1&amp;A2&amp;$C$1&amp;"]="&amp;$B$1&amp;"["&amp;B2&amp;"]"</f>
+        <v>mip_start["vInventory"]=output_rfep[1]</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C9" si="0">"mip_start["&amp;$C$1&amp;A3&amp;$C$1&amp;"]="&amp;$B$1&amp;"["&amp;B3&amp;"]"</f>
+        <v>mip_start["vRefuelQuantity"]=output_rfep[23]</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>mip_start["vRefuel"]=output_rfep[24]</v>
+      </c>
+      <c r="H4">
+        <f>H3+1</f>
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>mip_start["vQuantityUnitsCapacity"]=output_rfep[4]</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H31" si="1">H4+1</f>
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>mip_start["vLocate"]=output_rfep[5]</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>mip_start["vQuantityPurchased"]=output_rfep[6]</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>mip_start["vQuantityPurchasedRange"]=output_rfep[7]</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>mip_start["vPurchasedRange"]=output_rfep[8]</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I23" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I25" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I30" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I31" t="s">
+        <v>320</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C77"/>
@@ -6711,7 +7218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G32"/>
@@ -7230,13 +7737,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G36"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8204,12 +8711,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54D8714-998C-4B41-905B-35650263B8F4}">
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8487,7 +8994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G36"/>
@@ -9491,7 +9998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F43"/>
@@ -9978,7 +10485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G32"/>
@@ -10499,152 +11006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" t="str">
-        <f>B2&amp;"="&amp;$D$1&amp;"["&amp;A2&amp;"]"</f>
-        <v>sNodesVehiclesPaths2=output_domain_reduction[0]</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D9" si="0">B3&amp;"="&amp;$D$1&amp;"["&amp;A3&amp;"]"</f>
-        <v>sStationsVehiclesPaths2=output_domain_reduction[1]</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>sSequenceNodesNodesVehiclesPaths2=output_domain_reduction[2]</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>sFirstStationVehiclesPaths2=output_domain_reduction[3]</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>sNotFirstStationVehiclesPaths2=output_domain_reduction[4]</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>sNodesPotentialNodesOriginalVehiclesPaths2=output_domain_reduction[5]</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>pConsumptionMainRoute2=output_domain_reduction[6]</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>sStationsPaths2=output_domain_reduction[7]</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8792194EFF3EC4B9DEDA9143FB158AB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74d6161c0732f6a6a47db9602d75fed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6d2cdb912d1a107b914756c6dc16714" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10839,32 +11201,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00C25CB2-CB7D-473C-8D2E-8B42FDF875CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10881,4 +11236,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix the start_mip logic I reconfigured the calculation of the summarized variables
</commit_message>
<xml_diff>
--- a/models/rfep elements.xlsx
+++ b/models/rfep elements.xlsx
@@ -8,28 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/j_callesalazar_deakin_edu_au/Documents/calle test/Disun Applications/Gurobi Applications/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="603" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{211BD5DB-49E1-401E-82F8-A0A5DC112343}"/>
+  <xr:revisionPtr revIDLastSave="644" documentId="11_EE1C295A38DA22C4232790138295884FB906F14C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7237496C-7E08-457D-A9E2-DE2A34CDD08A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="850" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model elements" sheetId="1" r:id="rId1"/>
     <sheet name="mip_start" sheetId="22" r:id="rId2"/>
     <sheet name="rfep after domain reduction" sheetId="3" r:id="rId3"/>
     <sheet name="output subproblem" sheetId="2" r:id="rId4"/>
-    <sheet name="Print Solution Function" sheetId="4" r:id="rId5"/>
-    <sheet name="rfep_output_readability" sheetId="21" r:id="rId6"/>
-    <sheet name="Domain reduction function" sheetId="6" r:id="rId7"/>
-    <sheet name="Function Read instance" sheetId="9" r:id="rId8"/>
-    <sheet name="output subproblem readability" sheetId="5" r:id="rId9"/>
-    <sheet name="output domain reduction" sheetId="8" r:id="rId10"/>
-    <sheet name="solve_multiple_frvrp" sheetId="10" r:id="rId11"/>
-    <sheet name="rfep run experiments" sheetId="13" r:id="rId12"/>
-    <sheet name="Print Solution Experiments" sheetId="14" r:id="rId13"/>
-    <sheet name="Building factor combination" sheetId="15" r:id="rId14"/>
-    <sheet name="Tracking events data reading" sheetId="16" r:id="rId15"/>
-    <sheet name="Tracking events solve multiple" sheetId="17" r:id="rId16"/>
-    <sheet name="Solution Methodologies" sheetId="20" r:id="rId17"/>
+    <sheet name="Print output rfep csv" sheetId="23" r:id="rId5"/>
+    <sheet name="Print Solution Function" sheetId="4" r:id="rId6"/>
+    <sheet name="rfep_output_readability" sheetId="21" r:id="rId7"/>
+    <sheet name="Domain reduction function" sheetId="6" r:id="rId8"/>
+    <sheet name="Function Read instance" sheetId="9" r:id="rId9"/>
+    <sheet name="output subproblem readability" sheetId="5" r:id="rId10"/>
+    <sheet name="output domain reduction" sheetId="8" r:id="rId11"/>
+    <sheet name="solve_multiple_frvrp" sheetId="10" r:id="rId12"/>
+    <sheet name="rfep run experiments" sheetId="13" r:id="rId13"/>
+    <sheet name="Print Solution Experiments" sheetId="14" r:id="rId14"/>
+    <sheet name="Building factor combination" sheetId="15" r:id="rId15"/>
+    <sheet name="Tracking events data reading" sheetId="16" r:id="rId16"/>
+    <sheet name="Tracking events solve multiple" sheetId="17" r:id="rId17"/>
+    <sheet name="Solution Methodologies" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="335">
   <si>
     <t>sets</t>
   </si>
@@ -1084,6 +1085,45 @@
   </si>
   <si>
     <t>Output</t>
+  </si>
+  <si>
+    <t>ls_data_rfep</t>
+  </si>
+  <si>
+    <t>ls_scenario_name</t>
+  </si>
+  <si>
+    <t>ls_solution_algorithm</t>
+  </si>
+  <si>
+    <t>ls_output_solve</t>
+  </si>
+  <si>
+    <t>b_print_refuelling_detail</t>
+  </si>
+  <si>
+    <t>b_print_refuelling_summary</t>
+  </si>
+  <si>
+    <t>b_print_location_summary</t>
+  </si>
+  <si>
+    <t>ls_total_time</t>
+  </si>
+  <si>
+    <t>di_event_read</t>
+  </si>
+  <si>
+    <t>di_process_duration_read</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Default val</t>
+  </si>
+  <si>
+    <t>Call</t>
   </si>
 </sst>
 </file>
@@ -2461,6 +2501,527 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="16" t="str">
+        <f>B2&amp;","</f>
+        <v>status,</v>
+      </c>
+      <c r="D2" s="18" t="str">
+        <f>"d_subproblem_"&amp;B2&amp;" = {}"</f>
+        <v>d_subproblem_status = {}</v>
+      </c>
+      <c r="E2" t="str">
+        <f>B2&amp;" = output_solve["&amp;A2&amp;"]"</f>
+        <v>status = output_solve[0]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f t="shared" ref="C3:C21" si="0">B3&amp;","</f>
+        <v>ovInventory,</v>
+      </c>
+      <c r="D3" s="18" t="str">
+        <f t="shared" ref="D3:D21" si="1">"d_subproblem_"&amp;B3&amp;" = {}"</f>
+        <v>d_subproblem_ovInventory = {}</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E21" si="2">B3&amp;" = output_solve["&amp;A3&amp;"]"</f>
+        <v>ovInventory = output_solve[1]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovRefuelQuantity,</v>
+      </c>
+      <c r="D4" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovRefuelQuantity = {}</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>ovRefuelQuantity = output_solve[2]</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovRefuel,</v>
+      </c>
+      <c r="D5" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovRefuel = {}</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>ovRefuel = output_solve[3]</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovQuantityUnitsCapacity,</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovQuantityUnitsCapacity = {}</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>ovQuantityUnitsCapacity = output_solve[4]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovLocate,</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovLocate = {}</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>ovLocate = output_solve[5]</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>6</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovQuantityPurchased,</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovQuantityPurchased = {}</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>ovQuantityPurchased = output_solve[6]</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovQuantityPurchasedRange,</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovQuantityPurchasedRange = {}</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>ovQuantityPurchasedRange = output_solve[7]</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>ovPurchasedRange,</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_ovPurchasedRange = {}</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>ovPurchasedRange = output_solve[8]</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>oTotalRefuellingCost,</v>
+      </c>
+      <c r="D11" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_oTotalRefuellingCost = {}</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>oTotalRefuellingCost = output_solve[9]</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>10</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>oTotalLocationCost,</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_oTotalLocationCost = {}</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>oTotalLocationCost = output_solve[10]</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>oTotalDiscount,</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_oTotalDiscount = {}</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>oTotalDiscount = output_solve[11]</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>oTotalCost,</v>
+      </c>
+      <c r="D14" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_oTotalCost = {}</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>oTotalCost = output_solve[12]</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <f>+A14+1</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>n_constraints,</v>
+      </c>
+      <c r="D15" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_n_constraints = {}</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>n_constraints = output_solve[13]</v>
+      </c>
+      <c r="G15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <f t="shared" ref="A16:A21" si="3">+A15+1</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>n_variables,</v>
+      </c>
+      <c r="D16" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_n_variables = {}</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>n_variables = output_solve[14]</v>
+      </c>
+      <c r="G16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>n_integer_variables,</v>
+      </c>
+      <c r="D17" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_n_integer_variables = {}</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>n_integer_variables = output_solve[15]</v>
+      </c>
+      <c r="G17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>n_binary_variables,</v>
+      </c>
+      <c r="D18" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_n_binary_variables = {}</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>n_binary_variables = output_solve[16]</v>
+      </c>
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>model_fingerprint,</v>
+      </c>
+      <c r="D19" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_model_fingerprint = {}</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>model_fingerprint = output_solve[17]</v>
+      </c>
+      <c r="G19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>model_runtime,</v>
+      </c>
+      <c r="D20" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_model_runtime = {}</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>model_runtime = output_solve[18]</v>
+      </c>
+      <c r="G20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>model_MIPGap,</v>
+      </c>
+      <c r="D21" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>d_subproblem_model_MIPGap = {}</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>model_MIPGap = output_solve[19]</v>
+      </c>
+      <c r="G21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="G22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D9"/>
@@ -2587,7 +3148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F26CE2-C90F-4A38-9A6A-C140B73B9CCE}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:C35"/>
@@ -3051,7 +3612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B35F91-3CD2-4C06-9BDF-CB9DD17C3DF6}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C70"/>
@@ -3962,7 +4523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7958CFEE-249C-447C-B869-76486DCAFC59}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:F34"/>
@@ -4645,7 +5206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F78C82-2E64-4261-A67D-49932A4E459B}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:O19"/>
@@ -5021,7 +5582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CF5A27-5F77-4909-AEA0-BD4A0A79DDCF}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:G37"/>
@@ -5766,7 +6327,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F50D163-8D8F-40C3-B1E6-F806996DCA94}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:G5"/>
@@ -5874,7 +6435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121D905D-4443-4D4F-BAC5-5F82C02E29B9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5929,7 +6490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C04E18-08DD-4053-843A-816A92C25787}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
@@ -7738,12 +8299,204 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586278A8-0950-4040-A2E3-4774E7D6A7BA}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"False"</f>
+        <v>False</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"False"</f>
+        <v>False</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ref="B9:C12" si="0">"False"</f>
+        <v>False</v>
+      </c>
+      <c r="C9" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>False</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>328</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>False</v>
+      </c>
+      <c r="C11" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>False</v>
+      </c>
+      <c r="C12" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"True"</f>
+        <v>True</v>
+      </c>
+      <c r="C13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8711,7 +9464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54D8714-998C-4B41-905B-35650263B8F4}">
   <dimension ref="A1:B30"/>
   <sheetViews>
@@ -8994,7 +9747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G36"/>
@@ -9998,7 +10751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:F43"/>
@@ -10485,528 +11238,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:G32"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="83.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
-        <v>0</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="16" t="str">
-        <f>B2&amp;","</f>
-        <v>status,</v>
-      </c>
-      <c r="D2" s="18" t="str">
-        <f>"d_subproblem_"&amp;B2&amp;" = {}"</f>
-        <v>d_subproblem_status = {}</v>
-      </c>
-      <c r="E2" t="str">
-        <f>B2&amp;" = output_solve["&amp;A2&amp;"]"</f>
-        <v>status = output_solve[0]</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="16" t="str">
-        <f t="shared" ref="C3:C21" si="0">B3&amp;","</f>
-        <v>ovInventory,</v>
-      </c>
-      <c r="D3" s="18" t="str">
-        <f t="shared" ref="D3:D21" si="1">"d_subproblem_"&amp;B3&amp;" = {}"</f>
-        <v>d_subproblem_ovInventory = {}</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E21" si="2">B3&amp;" = output_solve["&amp;A3&amp;"]"</f>
-        <v>ovInventory = output_solve[1]</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovRefuelQuantity,</v>
-      </c>
-      <c r="D4" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovRefuelQuantity = {}</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="2"/>
-        <v>ovRefuelQuantity = output_solve[2]</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovRefuel,</v>
-      </c>
-      <c r="D5" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovRefuel = {}</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="2"/>
-        <v>ovRefuel = output_solve[3]</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>4</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovQuantityUnitsCapacity,</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovQuantityUnitsCapacity = {}</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="2"/>
-        <v>ovQuantityUnitsCapacity = output_solve[4]</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
-        <v>5</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovLocate,</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovLocate = {}</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="2"/>
-        <v>ovLocate = output_solve[5]</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>6</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovQuantityPurchased,</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovQuantityPurchased = {}</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="2"/>
-        <v>ovQuantityPurchased = output_solve[6]</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>7</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovQuantityPurchasedRange,</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovQuantityPurchasedRange = {}</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="2"/>
-        <v>ovQuantityPurchasedRange = output_solve[7]</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>8</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>ovPurchasedRange,</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_ovPurchasedRange = {}</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="2"/>
-        <v>ovPurchasedRange = output_solve[8]</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
-        <v>9</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>oTotalRefuellingCost,</v>
-      </c>
-      <c r="D11" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_oTotalRefuellingCost = {}</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="2"/>
-        <v>oTotalRefuellingCost = output_solve[9]</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>10</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>oTotalLocationCost,</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_oTotalLocationCost = {}</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="2"/>
-        <v>oTotalLocationCost = output_solve[10]</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
-        <v>11</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>oTotalDiscount,</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_oTotalDiscount = {}</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="2"/>
-        <v>oTotalDiscount = output_solve[11]</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>12</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v>oTotalCost,</v>
-      </c>
-      <c r="D14" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_oTotalCost = {}</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="2"/>
-        <v>oTotalCost = output_solve[12]</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
-        <f>+A14+1</f>
-        <v>13</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>n_constraints,</v>
-      </c>
-      <c r="D15" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_n_constraints = {}</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="2"/>
-        <v>n_constraints = output_solve[13]</v>
-      </c>
-      <c r="G15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
-        <f t="shared" ref="A16:A21" si="3">+A15+1</f>
-        <v>14</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>n_variables,</v>
-      </c>
-      <c r="D16" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_n_variables = {}</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="2"/>
-        <v>n_variables = output_solve[14]</v>
-      </c>
-      <c r="G16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>n_integer_variables,</v>
-      </c>
-      <c r="D17" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_n_integer_variables = {}</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="2"/>
-        <v>n_integer_variables = output_solve[15]</v>
-      </c>
-      <c r="G17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
-        <f t="shared" si="3"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>n_binary_variables,</v>
-      </c>
-      <c r="D18" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_n_binary_variables = {}</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="2"/>
-        <v>n_binary_variables = output_solve[16]</v>
-      </c>
-      <c r="G18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
-        <f t="shared" si="3"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>model_fingerprint,</v>
-      </c>
-      <c r="D19" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_model_fingerprint = {}</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="2"/>
-        <v>model_fingerprint = output_solve[17]</v>
-      </c>
-      <c r="G19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>model_runtime,</v>
-      </c>
-      <c r="D20" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_model_runtime = {}</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="2"/>
-        <v>model_runtime = output_solve[18]</v>
-      </c>
-      <c r="G20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
-        <f t="shared" si="3"/>
-        <v>19</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>model_MIPGap,</v>
-      </c>
-      <c r="D21" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>d_subproblem_model_MIPGap = {}</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="2"/>
-        <v>model_MIPGap = output_solve[19]</v>
-      </c>
-      <c r="G21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="G22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8792194EFF3EC4B9DEDA9143FB158AB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74d6161c0732f6a6a47db9602d75fed5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6d2cdb912d1a107b914756c6dc16714" ns1:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11201,25 +11451,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00C25CB2-CB7D-473C-8D2E-8B42FDF875CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11236,29 +11493,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70947567-7DC9-47DC-850B-2CD1F71865E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A7B44E1-5F82-4F69-A389-4E8AF5DC0F08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="06cfa1d4-1421-4afe-8ba9-b40c17f3ba4c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>